<commit_message>
user fixes. createuser command
</commit_message>
<xml_diff>
--- a/priceTrackerTables.xlsx
+++ b/priceTrackerTables.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\django\priceTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3E66BB-02BA-4E12-811F-6CD29B6A924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576D11BB-9C7C-4E56-87C7-DBC354212CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="690" windowWidth="21600" windowHeight="14910" xr2:uid="{A0984463-1538-4671-813D-D6CC57BDADC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A0984463-1538-4671-813D-D6CC57BDADC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
     <sheet name="Fields" sheetId="3" r:id="rId2"/>
-    <sheet name="Values" sheetId="4" r:id="rId3"/>
-    <sheet name="main" sheetId="2" r:id="rId4"/>
-    <sheet name="price_menu" sheetId="5" r:id="rId5"/>
-    <sheet name="food" sheetId="7" r:id="rId6"/>
-    <sheet name="food_prices" sheetId="6" r:id="rId7"/>
+    <sheet name="QueryService" sheetId="8" r:id="rId3"/>
+    <sheet name="Values" sheetId="4" r:id="rId4"/>
+    <sheet name="main" sheetId="2" r:id="rId5"/>
+    <sheet name="price_menu" sheetId="5" r:id="rId6"/>
+    <sheet name="food" sheetId="7" r:id="rId7"/>
+    <sheet name="food_prices" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fields!$A$1:$F$164</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="262">
   <si>
     <t>Main</t>
   </si>
@@ -692,18 +693,12 @@
     <t>Sevices</t>
   </si>
   <si>
-    <t>Taxi Prices</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
     <t>Transport</t>
   </si>
   <si>
-    <t>Public TransportPrice</t>
-  </si>
-  <si>
     <t>GasolinePrice</t>
   </si>
   <si>
@@ -720,13 +715,127 @@
   </si>
   <si>
     <t>Mvp</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>The query service is needed to produce tables and charts</t>
+  </si>
+  <si>
+    <t>A set of json queries are provided</t>
+  </si>
+  <si>
+    <t>table : food</t>
+  </si>
+  <si>
+    <t>form_date : 01/01/2020</t>
+  </si>
+  <si>
+    <t>to_date : 01/01/2021</t>
+  </si>
+  <si>
+    <t>column : "avg(price)"</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>The service returns a the results as a table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data is partitioned into columns ( x ) and rows ( y) </t>
+  </si>
+  <si>
+    <t>{ country , state , city , year , month, week , day }</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from </t>
+  </si>
+  <si>
+    <t>{table}</t>
+  </si>
+  <si>
+    <t>for p in Person.objects.raw('SELECT * FROM myapp_person'):</t>
+  </si>
+  <si>
+    <t>where</t>
+  </si>
+  <si>
+    <t>date between {from_date} and {to_date}</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>country in {country_list}</t>
+  </si>
+  <si>
+    <t>country_list</t>
+  </si>
+  <si>
+    <t>state in {state_list}</t>
+  </si>
+  <si>
+    <t>city in {city_list}</t>
+  </si>
+  <si>
+    <t>group by { x, y}</t>
+  </si>
+  <si>
+    <t>{x}, {y},{column}</t>
+  </si>
+  <si>
+    <t>I need a model with the following structure</t>
+  </si>
+  <si>
+    <t>dim1</t>
+  </si>
+  <si>
+    <t>dim2</t>
+  </si>
+  <si>
+    <t>dim3</t>
+  </si>
+  <si>
+    <t>value01</t>
+  </si>
+  <si>
+    <t>def pivot (data)</t>
+  </si>
+  <si>
+    <t>Then , the result has to be pivoted with x as columns</t>
+  </si>
+  <si>
+    <t>sort data by {x} , {y}</t>
+  </si>
+  <si>
+    <t>This can also be done with postgresql crosstab function</t>
+  </si>
+  <si>
+    <t>https://www.postgresql.org/docs/current/tablefunc.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -756,6 +865,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="8">
@@ -868,7 +982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -892,6 +1006,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1206,71 +1324,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C77FEE-F832-43C4-A92B-CA75BC9DC9BF}">
-  <dimension ref="B1:L35"/>
+  <dimension ref="B1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="62.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13">
       <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>225</v>
-      </c>
       <c r="F1" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13">
       <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="14"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="14">
-        <v>1</v>
-      </c>
       <c r="I2" s="14">
         <v>1</v>
       </c>
@@ -1283,105 +1405,116 @@
       <c r="L2" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
       <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="14"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="14">
-        <v>1</v>
-      </c>
-      <c r="G3" s="14" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14">
+        <v>1</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
-      <c r="L3" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="14"/>
+      <c r="M3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13">
       <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="14"/>
       <c r="E4" s="14"/>
-      <c r="F4" s="14">
-        <v>1</v>
-      </c>
-      <c r="G4" s="14" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14">
+        <v>1</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
-      <c r="L4" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="14"/>
+      <c r="M4" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13">
       <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
-      <c r="L5" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="14"/>
+      <c r="M5" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
       <c r="B6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="14">
-        <v>1</v>
-      </c>
-      <c r="G6" s="14" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14">
+        <v>1</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
-      <c r="L6" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="14"/>
+      <c r="M6" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
       <c r="B7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -1389,18 +1522,19 @@
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
-      <c r="L7" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="14"/>
+      <c r="M7" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -1408,256 +1542,269 @@
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
-      <c r="L8" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="14"/>
+      <c r="M8" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
       <c r="B9" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="14"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="14">
-        <v>1</v>
-      </c>
-      <c r="G9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14">
+        <v>1</v>
+      </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="14"/>
+      <c r="M9" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
       <c r="B10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="14"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14">
+        <v>1</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="14"/>
+      <c r="M10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13">
       <c r="B11" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="15"/>
       <c r="E11" s="15"/>
-      <c r="F11" s="15">
-        <v>1</v>
-      </c>
-      <c r="G11" s="15" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="15">
+        <v>1</v>
+      </c>
+      <c r="H11" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15">
-        <v>1</v>
-      </c>
-      <c r="J11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15">
+        <v>1</v>
+      </c>
       <c r="K11" s="15"/>
-      <c r="L11" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L11" s="15"/>
+      <c r="M11" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
       <c r="B12" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="15"/>
       <c r="E12" s="15"/>
-      <c r="F12" s="15">
-        <v>1</v>
-      </c>
-      <c r="G12" s="15" t="s">
+      <c r="F12" s="15"/>
+      <c r="G12" s="15">
+        <v>1</v>
+      </c>
+      <c r="H12" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15">
-        <v>1</v>
-      </c>
-      <c r="J12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15">
+        <v>1</v>
+      </c>
       <c r="K12" s="15"/>
-      <c r="L12" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L12" s="15"/>
+      <c r="M12" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
       <c r="B13" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="15"/>
+      <c r="D13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="15"/>
       <c r="E13" s="15"/>
-      <c r="F13" s="15">
-        <v>1</v>
-      </c>
-      <c r="G13" s="15" t="s">
+      <c r="F13" s="15"/>
+      <c r="G13" s="15">
+        <v>1</v>
+      </c>
+      <c r="H13" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="15"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
-      <c r="L13" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="15"/>
+      <c r="M13" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
       <c r="B14" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="15"/>
       <c r="E14" s="15"/>
-      <c r="F14" s="15">
-        <v>1</v>
-      </c>
-      <c r="G14" s="15" t="s">
+      <c r="F14" s="15"/>
+      <c r="G14" s="15">
+        <v>1</v>
+      </c>
+      <c r="H14" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15">
-        <v>1</v>
-      </c>
-      <c r="J14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15">
+        <v>1</v>
+      </c>
       <c r="K14" s="15"/>
-      <c r="L14" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L14" s="15"/>
+      <c r="M14" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
       <c r="B15" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="15"/>
       <c r="E15" s="15"/>
-      <c r="F15" s="15">
-        <v>1</v>
-      </c>
-      <c r="G15" s="15" t="s">
+      <c r="F15" s="15"/>
+      <c r="G15" s="15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15">
-        <v>1</v>
-      </c>
-      <c r="J15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15">
+        <v>1</v>
+      </c>
       <c r="K15" s="15"/>
-      <c r="L15" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="15"/>
+      <c r="M15" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
       <c r="B16" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="15"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="15">
-        <v>1</v>
-      </c>
-      <c r="G16" s="15" t="s">
+      <c r="F16" s="15"/>
+      <c r="G16" s="15">
+        <v>1</v>
+      </c>
+      <c r="H16" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15">
-        <v>1</v>
-      </c>
-      <c r="J16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15">
+        <v>1</v>
+      </c>
       <c r="K16" s="15"/>
-      <c r="L16" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L16" s="15"/>
+      <c r="M16" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
       <c r="B17" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="15"/>
+      <c r="D17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="15"/>
       <c r="E17" s="15"/>
-      <c r="F17" s="15">
-        <v>1</v>
-      </c>
-      <c r="G17" s="15" t="s">
+      <c r="F17" s="15"/>
+      <c r="G17" s="15">
+        <v>1</v>
+      </c>
+      <c r="H17" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
-      <c r="L17" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="15"/>
+      <c r="M17" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
       <c r="B18" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="15"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="15">
-        <v>1</v>
-      </c>
-      <c r="G18" s="15" t="s">
+      <c r="F18" s="15"/>
+      <c r="G18" s="15">
+        <v>1</v>
+      </c>
+      <c r="H18" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15">
-        <v>1</v>
-      </c>
-      <c r="J18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15">
+        <v>1</v>
+      </c>
       <c r="K18" s="15"/>
-      <c r="L18" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L18" s="15"/>
+      <c r="M18" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
       <c r="B19" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
@@ -1665,113 +1812,124 @@
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
-      <c r="L19" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L19" s="15"/>
+      <c r="M19" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
       <c r="B20" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="15"/>
+      <c r="D20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="15"/>
       <c r="E20" s="15"/>
-      <c r="F20" s="15">
-        <v>1</v>
-      </c>
-      <c r="G20" s="15" t="s">
+      <c r="F20" s="15"/>
+      <c r="G20" s="15">
+        <v>1</v>
+      </c>
+      <c r="H20" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15">
-        <v>1</v>
-      </c>
-      <c r="J20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15">
+        <v>1</v>
+      </c>
       <c r="K20" s="15"/>
-      <c r="L20" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L20" s="15"/>
+      <c r="M20" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13">
       <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5" t="s">
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L21" s="5"/>
+      <c r="M21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
       <c r="B22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="5">
-        <v>1</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5" t="s">
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13">
       <c r="B23" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="5">
-        <v>1</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5" t="s">
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13">
       <c r="B24" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="C24" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -1779,60 +1937,69 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13">
       <c r="B25" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="5">
-        <v>1</v>
-      </c>
-      <c r="F25" s="5"/>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13">
       <c r="B26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E26" s="5">
-        <v>1</v>
-      </c>
-      <c r="F26" s="5"/>
+      <c r="E26" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13">
       <c r="B27" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
@@ -1840,18 +2007,21 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13">
       <c r="B28" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="C28" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -1859,18 +2029,21 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13">
       <c r="B29" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="C29" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -1878,37 +2051,45 @@
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13">
       <c r="B30" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C30" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13">
       <c r="B31" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C31" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -1916,85 +2097,74 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13">
       <c r="B32" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C32" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F32" s="5">
+        <v>1</v>
+      </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="E33" s="5">
-        <v>1</v>
-      </c>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="16" t="s">
+      <c r="M32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13">
+      <c r="B33" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C33" s="16"/>
+      <c r="D33" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16" t="s">
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:L35">
-    <sortCondition ref="C2:C35"/>
-    <sortCondition ref="B2:B35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:M34">
+    <sortCondition ref="D2:D34"/>
+    <sortCondition ref="B2:B34"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2007,10 +2177,10 @@
   <dimension ref="A1:F164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
@@ -2020,7 +2190,7 @@
     <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -2040,7 +2210,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -2060,7 +2230,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -2078,7 +2248,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -2096,7 +2266,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -2114,7 +2284,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -2132,7 +2302,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -2150,7 +2320,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1">
       <c r="A8" s="5" t="s">
         <v>201</v>
       </c>
@@ -2160,7 +2330,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1">
       <c r="A9" s="5" t="s">
         <v>201</v>
       </c>
@@ -2180,7 +2350,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -2192,7 +2362,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
@@ -2212,7 +2382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -2232,7 +2402,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1">
       <c r="A13" s="5" t="s">
         <v>83</v>
       </c>
@@ -2244,7 +2414,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1">
       <c r="A14" s="5" t="s">
         <v>83</v>
       </c>
@@ -2264,7 +2434,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1">
       <c r="A15" s="5" t="s">
         <v>83</v>
       </c>
@@ -2284,7 +2454,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1">
       <c r="A16" s="5" t="s">
         <v>83</v>
       </c>
@@ -2304,7 +2474,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1">
       <c r="A17" s="5" t="s">
         <v>83</v>
       </c>
@@ -2322,7 +2492,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1">
       <c r="A18" s="5" t="s">
         <v>8</v>
       </c>
@@ -2334,7 +2504,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
@@ -2354,7 +2524,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1">
       <c r="A20" s="5" t="s">
         <v>8</v>
       </c>
@@ -2374,7 +2544,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1">
       <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
@@ -2392,7 +2562,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -2410,7 +2580,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1">
       <c r="A23" s="5" t="s">
         <v>8</v>
       </c>
@@ -2428,7 +2598,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -2446,7 +2616,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1">
       <c r="A25" s="5" t="s">
         <v>8</v>
       </c>
@@ -2464,7 +2634,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
@@ -2476,7 +2646,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1">
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
@@ -2496,7 +2666,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1">
       <c r="A28" s="5" t="s">
         <v>9</v>
       </c>
@@ -2514,7 +2684,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1">
       <c r="A29" s="5" t="s">
         <v>9</v>
       </c>
@@ -2532,7 +2702,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1">
       <c r="A30" s="5" t="s">
         <v>9</v>
       </c>
@@ -2550,7 +2720,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1">
       <c r="A31" s="5" t="s">
         <v>10</v>
       </c>
@@ -2562,7 +2732,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1">
       <c r="A32" s="5" t="s">
         <v>10</v>
       </c>
@@ -2582,7 +2752,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1">
       <c r="A33" s="5" t="s">
         <v>10</v>
       </c>
@@ -2600,7 +2770,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1">
       <c r="A34" s="5" t="s">
         <v>11</v>
       </c>
@@ -2612,7 +2782,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1">
       <c r="A35" s="5" t="s">
         <v>11</v>
       </c>
@@ -2630,7 +2800,7 @@
       </c>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1">
       <c r="A36" s="5" t="s">
         <v>11</v>
       </c>
@@ -2648,7 +2818,7 @@
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1">
       <c r="A37" s="5" t="s">
         <v>11</v>
       </c>
@@ -2666,7 +2836,7 @@
       </c>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1">
       <c r="A38" s="5" t="s">
         <v>11</v>
       </c>
@@ -2684,7 +2854,7 @@
       </c>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1">
       <c r="A39" s="5" t="s">
         <v>11</v>
       </c>
@@ -2698,7 +2868,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1">
       <c r="A40" s="5" t="s">
         <v>13</v>
       </c>
@@ -2710,7 +2880,7 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1">
       <c r="A41" s="5" t="s">
         <v>13</v>
       </c>
@@ -2730,7 +2900,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1">
       <c r="A42" s="5" t="s">
         <v>13</v>
       </c>
@@ -2750,7 +2920,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1">
       <c r="A43" s="5" t="s">
         <v>13</v>
       </c>
@@ -2770,7 +2940,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1">
       <c r="A44" s="5" t="s">
         <v>13</v>
       </c>
@@ -2790,7 +2960,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1">
       <c r="A45" s="5" t="s">
         <v>13</v>
       </c>
@@ -2808,7 +2978,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1">
       <c r="A46" s="5" t="s">
         <v>13</v>
       </c>
@@ -2826,7 +2996,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1">
       <c r="A47" s="5" t="s">
         <v>13</v>
       </c>
@@ -2842,7 +3012,7 @@
       </c>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1">
       <c r="A48" s="5" t="s">
         <v>13</v>
       </c>
@@ -2858,7 +3028,7 @@
       </c>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1">
       <c r="A49" s="5" t="s">
         <v>13</v>
       </c>
@@ -2876,7 +3046,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1">
       <c r="A50" s="5" t="s">
         <v>13</v>
       </c>
@@ -2894,7 +3064,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1">
       <c r="A51" s="5" t="s">
         <v>13</v>
       </c>
@@ -2912,7 +3082,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1">
       <c r="A52" s="5" t="s">
         <v>13</v>
       </c>
@@ -2930,7 +3100,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1">
       <c r="A53" s="5" t="s">
         <v>14</v>
       </c>
@@ -2942,7 +3112,7 @@
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1">
       <c r="A54" s="5" t="s">
         <v>14</v>
       </c>
@@ -2962,7 +3132,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1">
       <c r="A55" s="5" t="s">
         <v>14</v>
       </c>
@@ -2980,7 +3150,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1">
       <c r="A56" s="5" t="s">
         <v>14</v>
       </c>
@@ -2996,7 +3166,7 @@
       </c>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1">
       <c r="A57" s="5" t="s">
         <v>14</v>
       </c>
@@ -3012,7 +3182,7 @@
       </c>
       <c r="F57" s="5"/>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1">
       <c r="A58" s="5" t="s">
         <v>14</v>
       </c>
@@ -3030,7 +3200,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1">
       <c r="A59" s="5" t="s">
         <v>14</v>
       </c>
@@ -3048,7 +3218,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1">
       <c r="A60" s="5" t="s">
         <v>14</v>
       </c>
@@ -3066,7 +3236,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1">
       <c r="A61" s="5" t="s">
         <v>14</v>
       </c>
@@ -3082,7 +3252,7 @@
       </c>
       <c r="F61" s="5"/>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1">
       <c r="A62" s="5" t="s">
         <v>14</v>
       </c>
@@ -3098,7 +3268,7 @@
       </c>
       <c r="F62" s="5"/>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1">
       <c r="A63" s="5" t="s">
         <v>14</v>
       </c>
@@ -3114,7 +3284,7 @@
       </c>
       <c r="F63" s="5"/>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1">
       <c r="A64" s="5" t="s">
         <v>14</v>
       </c>
@@ -3130,7 +3300,7 @@
       </c>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1">
       <c r="A65" s="5" t="s">
         <v>135</v>
       </c>
@@ -3142,7 +3312,7 @@
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" hidden="1">
       <c r="A66" s="5" t="s">
         <v>135</v>
       </c>
@@ -3158,7 +3328,7 @@
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" hidden="1">
       <c r="A67" s="5" t="s">
         <v>135</v>
       </c>
@@ -3176,7 +3346,7 @@
       </c>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" hidden="1">
       <c r="A68" s="5" t="s">
         <v>135</v>
       </c>
@@ -3192,7 +3362,7 @@
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" hidden="1">
       <c r="A69" s="5" t="s">
         <v>135</v>
       </c>
@@ -3206,7 +3376,7 @@
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" hidden="1">
       <c r="A70" s="5" t="s">
         <v>135</v>
       </c>
@@ -3220,7 +3390,7 @@
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1">
       <c r="A71" s="5" t="s">
         <v>135</v>
       </c>
@@ -3234,7 +3404,7 @@
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" hidden="1">
       <c r="A72" s="5" t="s">
         <v>135</v>
       </c>
@@ -3248,7 +3418,7 @@
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" hidden="1">
       <c r="A73" s="5" t="s">
         <v>137</v>
       </c>
@@ -3260,7 +3430,7 @@
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" hidden="1">
       <c r="A74" s="5" t="s">
         <v>137</v>
       </c>
@@ -3278,7 +3448,7 @@
       </c>
       <c r="F74" s="5"/>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" hidden="1">
       <c r="A75" s="5" t="s">
         <v>137</v>
       </c>
@@ -3292,7 +3462,7 @@
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1">
       <c r="A76" s="5" t="s">
         <v>137</v>
       </c>
@@ -3308,7 +3478,7 @@
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" hidden="1">
       <c r="A77" s="5" t="s">
         <v>137</v>
       </c>
@@ -3324,7 +3494,7 @@
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" hidden="1">
       <c r="A78" s="5" t="s">
         <v>137</v>
       </c>
@@ -3340,7 +3510,7 @@
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" hidden="1">
       <c r="A79" s="5" t="s">
         <v>16</v>
       </c>
@@ -3350,7 +3520,7 @@
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" hidden="1">
       <c r="A80" s="5" t="s">
         <v>16</v>
       </c>
@@ -3366,7 +3536,7 @@
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1">
       <c r="A81" s="5" t="s">
         <v>16</v>
       </c>
@@ -3382,7 +3552,7 @@
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1">
       <c r="A82" s="5" t="s">
         <v>16</v>
       </c>
@@ -3398,7 +3568,7 @@
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1">
       <c r="A83" s="5" t="s">
         <v>16</v>
       </c>
@@ -3414,7 +3584,7 @@
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" hidden="1">
       <c r="A84" s="5" t="s">
         <v>16</v>
       </c>
@@ -3430,7 +3600,7 @@
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" hidden="1">
       <c r="A85" s="5" t="s">
         <v>16</v>
       </c>
@@ -3448,7 +3618,7 @@
       </c>
       <c r="F85" s="5"/>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" hidden="1">
       <c r="A86" s="5" t="s">
         <v>16</v>
       </c>
@@ -3462,7 +3632,7 @@
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" hidden="1">
       <c r="A87" s="5" t="s">
         <v>16</v>
       </c>
@@ -3476,7 +3646,7 @@
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" hidden="1">
       <c r="A88" s="5" t="s">
         <v>16</v>
       </c>
@@ -3490,7 +3660,7 @@
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" hidden="1">
       <c r="A89" s="5" t="s">
         <v>16</v>
       </c>
@@ -3504,7 +3674,7 @@
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" hidden="1">
       <c r="A90" s="5" t="s">
         <v>16</v>
       </c>
@@ -3518,7 +3688,7 @@
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" hidden="1">
       <c r="A91" s="5" t="s">
         <v>16</v>
       </c>
@@ -3532,7 +3702,7 @@
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" hidden="1">
       <c r="A92" s="5" t="s">
         <v>145</v>
       </c>
@@ -3544,7 +3714,7 @@
       <c r="E92" s="5"/>
       <c r="F92" s="5"/>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" hidden="1">
       <c r="A93" s="5" t="s">
         <v>145</v>
       </c>
@@ -3558,7 +3728,7 @@
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" hidden="1">
       <c r="A94" s="5" t="s">
         <v>145</v>
       </c>
@@ -3572,7 +3742,7 @@
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" hidden="1">
       <c r="A95" s="5" t="s">
         <v>145</v>
       </c>
@@ -3586,7 +3756,7 @@
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1">
       <c r="A96" s="5" t="s">
         <v>145</v>
       </c>
@@ -3600,7 +3770,7 @@
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1">
       <c r="A97" s="5" t="s">
         <v>145</v>
       </c>
@@ -3614,7 +3784,7 @@
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1">
       <c r="A98" s="5" t="s">
         <v>145</v>
       </c>
@@ -3630,7 +3800,7 @@
       </c>
       <c r="F98" s="5"/>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1">
       <c r="A99" s="5" t="s">
         <v>145</v>
       </c>
@@ -3646,7 +3816,7 @@
       </c>
       <c r="F99" s="5"/>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1">
       <c r="A100" s="5" t="s">
         <v>145</v>
       </c>
@@ -3662,7 +3832,7 @@
       </c>
       <c r="F100" s="5"/>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1">
       <c r="A101" s="5" t="s">
         <v>145</v>
       </c>
@@ -3676,7 +3846,7 @@
       <c r="E101" s="5"/>
       <c r="F101" s="5"/>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1">
       <c r="A102" s="5" t="s">
         <v>145</v>
       </c>
@@ -3690,7 +3860,7 @@
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1">
       <c r="A103" s="5" t="s">
         <v>145</v>
       </c>
@@ -3704,7 +3874,7 @@
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1">
       <c r="A104" s="5" t="s">
         <v>145</v>
       </c>
@@ -3718,7 +3888,7 @@
       <c r="E104" s="5"/>
       <c r="F104" s="5"/>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1">
       <c r="A105" s="5" t="s">
         <v>145</v>
       </c>
@@ -3732,7 +3902,7 @@
       <c r="E105" s="5"/>
       <c r="F105" s="5"/>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1">
       <c r="A106" s="5" t="s">
         <v>145</v>
       </c>
@@ -3746,7 +3916,7 @@
       <c r="E106" s="5"/>
       <c r="F106" s="5"/>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1">
       <c r="A107" s="5" t="s">
         <v>145</v>
       </c>
@@ -3760,7 +3930,7 @@
       <c r="E107" s="5"/>
       <c r="F107" s="5"/>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1">
       <c r="A108" s="5" t="s">
         <v>145</v>
       </c>
@@ -3774,7 +3944,7 @@
       <c r="E108" s="5"/>
       <c r="F108" s="5"/>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1">
       <c r="A109" s="5" t="s">
         <v>145</v>
       </c>
@@ -3788,7 +3958,7 @@
       <c r="E109" s="5"/>
       <c r="F109" s="5"/>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1">
       <c r="A110" s="5" t="s">
         <v>145</v>
       </c>
@@ -3802,7 +3972,7 @@
       <c r="E110" s="5"/>
       <c r="F110" s="5"/>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1">
       <c r="A111" s="5" t="s">
         <v>145</v>
       </c>
@@ -3816,7 +3986,7 @@
       <c r="E111" s="5"/>
       <c r="F111" s="5"/>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1">
       <c r="A112" s="5" t="s">
         <v>145</v>
       </c>
@@ -3830,7 +4000,7 @@
       <c r="E112" s="5"/>
       <c r="F112" s="5"/>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1">
       <c r="A113" s="5" t="s">
         <v>145</v>
       </c>
@@ -3844,7 +4014,7 @@
       <c r="E113" s="5"/>
       <c r="F113" s="5"/>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1">
       <c r="A114" s="5" t="s">
         <v>145</v>
       </c>
@@ -3858,7 +4028,7 @@
       <c r="E114" s="5"/>
       <c r="F114" s="5"/>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1">
       <c r="A115" s="5" t="s">
         <v>72</v>
       </c>
@@ -3870,7 +4040,7 @@
       <c r="E115" s="5"/>
       <c r="F115" s="5"/>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1">
       <c r="A116" s="5" t="s">
         <v>72</v>
       </c>
@@ -3888,7 +4058,7 @@
       </c>
       <c r="F116" s="5"/>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1">
       <c r="A117" s="5" t="s">
         <v>72</v>
       </c>
@@ -3904,7 +4074,7 @@
       </c>
       <c r="F117" s="5"/>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1">
       <c r="A118" s="5" t="s">
         <v>72</v>
       </c>
@@ -3920,7 +4090,7 @@
       </c>
       <c r="F118" s="5"/>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1">
       <c r="A119" s="5" t="s">
         <v>18</v>
       </c>
@@ -3932,7 +4102,7 @@
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1">
       <c r="A120" s="5" t="s">
         <v>18</v>
       </c>
@@ -3950,7 +4120,7 @@
       </c>
       <c r="F120" s="5"/>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1">
       <c r="A121" s="5" t="s">
         <v>18</v>
       </c>
@@ -3966,7 +4136,7 @@
       </c>
       <c r="F121" s="5"/>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1">
       <c r="A122" s="5" t="s">
         <v>18</v>
       </c>
@@ -3982,7 +4152,7 @@
       </c>
       <c r="F122" s="5"/>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1">
       <c r="A123" s="5" t="s">
         <v>18</v>
       </c>
@@ -3998,7 +4168,7 @@
       </c>
       <c r="F123" s="5"/>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1">
       <c r="A124" s="5" t="s">
         <v>18</v>
       </c>
@@ -4014,7 +4184,7 @@
       </c>
       <c r="F124" s="5"/>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1">
       <c r="A125" s="5" t="s">
         <v>18</v>
       </c>
@@ -4030,7 +4200,7 @@
       </c>
       <c r="F125" s="5"/>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1">
       <c r="A126" s="5" t="s">
         <v>18</v>
       </c>
@@ -4046,7 +4216,7 @@
       </c>
       <c r="F126" s="5"/>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6">
       <c r="A127" s="5" t="s">
         <v>170</v>
       </c>
@@ -4058,7 +4228,7 @@
       <c r="E127" s="5"/>
       <c r="F127" s="5"/>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6">
       <c r="A128" s="5" t="s">
         <v>170</v>
       </c>
@@ -4074,7 +4244,7 @@
       <c r="E128" s="5"/>
       <c r="F128" s="5"/>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6">
       <c r="A129" s="5" t="s">
         <v>170</v>
       </c>
@@ -4088,7 +4258,7 @@
       <c r="E129" s="5"/>
       <c r="F129" s="5"/>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6">
       <c r="A130" s="5" t="s">
         <v>170</v>
       </c>
@@ -4102,7 +4272,7 @@
       <c r="E130" s="5"/>
       <c r="F130" s="5"/>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6">
       <c r="A131" s="5" t="s">
         <v>170</v>
       </c>
@@ -4116,7 +4286,7 @@
       <c r="E131" s="5"/>
       <c r="F131" s="5"/>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6">
       <c r="A132" s="5" t="s">
         <v>170</v>
       </c>
@@ -4132,7 +4302,7 @@
       </c>
       <c r="F132" s="5"/>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6">
       <c r="A133" s="5" t="s">
         <v>170</v>
       </c>
@@ -4148,7 +4318,7 @@
       </c>
       <c r="F133" s="5"/>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6">
       <c r="A134" s="5" t="s">
         <v>170</v>
       </c>
@@ -4164,7 +4334,7 @@
       </c>
       <c r="F134" s="5"/>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6">
       <c r="A135" s="5" t="s">
         <v>170</v>
       </c>
@@ -4178,7 +4348,7 @@
       <c r="E135" s="5"/>
       <c r="F135" s="5"/>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" hidden="1">
       <c r="A136" s="5" t="s">
         <v>19</v>
       </c>
@@ -4190,7 +4360,7 @@
       <c r="E136" s="5"/>
       <c r="F136" s="5"/>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" hidden="1">
       <c r="A137" s="5" t="s">
         <v>19</v>
       </c>
@@ -4204,7 +4374,7 @@
       <c r="E137" s="5"/>
       <c r="F137" s="5"/>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" hidden="1">
       <c r="A138" s="5" t="s">
         <v>19</v>
       </c>
@@ -4218,7 +4388,7 @@
       <c r="E138" s="5"/>
       <c r="F138" s="5"/>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" hidden="1">
       <c r="A139" s="5" t="s">
         <v>19</v>
       </c>
@@ -4234,7 +4404,7 @@
       </c>
       <c r="F139" s="5"/>
     </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" hidden="1">
       <c r="A140" s="5" t="s">
         <v>19</v>
       </c>
@@ -4250,7 +4420,7 @@
       </c>
       <c r="F140" s="5"/>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" hidden="1">
       <c r="A141" s="5" t="s">
         <v>19</v>
       </c>
@@ -4264,7 +4434,7 @@
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" hidden="1">
       <c r="A142" s="5" t="s">
         <v>24</v>
       </c>
@@ -4272,7 +4442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" hidden="1">
       <c r="A143" s="5" t="s">
         <v>24</v>
       </c>
@@ -4290,7 +4460,7 @@
       </c>
       <c r="F143" s="5"/>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" hidden="1">
       <c r="A144" s="5" t="s">
         <v>24</v>
       </c>
@@ -4308,7 +4478,7 @@
       </c>
       <c r="F144" s="5"/>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" hidden="1">
       <c r="A145" s="5" t="s">
         <v>24</v>
       </c>
@@ -4324,7 +4494,7 @@
       </c>
       <c r="F145" s="5"/>
     </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" hidden="1">
       <c r="A146" s="5" t="s">
         <v>24</v>
       </c>
@@ -4340,7 +4510,7 @@
       </c>
       <c r="F146" s="5"/>
     </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" hidden="1">
       <c r="A147" s="5" t="s">
         <v>24</v>
       </c>
@@ -4356,7 +4526,7 @@
       </c>
       <c r="F147" s="5"/>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" hidden="1">
       <c r="A148" s="5" t="s">
         <v>25</v>
       </c>
@@ -4368,7 +4538,7 @@
       <c r="E148" s="5"/>
       <c r="F148" s="5"/>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" hidden="1">
       <c r="A149" s="5" t="s">
         <v>25</v>
       </c>
@@ -4386,7 +4556,7 @@
       </c>
       <c r="F149" s="5"/>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" hidden="1">
       <c r="A150" s="5" t="s">
         <v>25</v>
       </c>
@@ -4402,7 +4572,7 @@
       </c>
       <c r="F150" s="5"/>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" hidden="1">
       <c r="A151" s="5" t="s">
         <v>25</v>
       </c>
@@ -4418,7 +4588,7 @@
       </c>
       <c r="F151" s="5"/>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" hidden="1">
       <c r="A152" s="5" t="s">
         <v>25</v>
       </c>
@@ -4434,7 +4604,7 @@
       </c>
       <c r="F152" s="5"/>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" hidden="1">
       <c r="A153" s="5" t="s">
         <v>178</v>
       </c>
@@ -4446,7 +4616,7 @@
       <c r="E153" s="5"/>
       <c r="F153" s="5"/>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" hidden="1">
       <c r="A154" s="5" t="s">
         <v>178</v>
       </c>
@@ -4462,7 +4632,7 @@
       </c>
       <c r="F154" s="5"/>
     </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" hidden="1">
       <c r="A155" s="5" t="s">
         <v>178</v>
       </c>
@@ -4478,7 +4648,7 @@
       </c>
       <c r="F155" s="5"/>
     </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" hidden="1">
       <c r="A156" s="5" t="s">
         <v>178</v>
       </c>
@@ -4494,7 +4664,7 @@
       </c>
       <c r="F156" s="5"/>
     </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" hidden="1">
       <c r="A157" s="5" t="s">
         <v>178</v>
       </c>
@@ -4510,7 +4680,7 @@
       </c>
       <c r="F157" s="5"/>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" hidden="1">
       <c r="A158" s="5" t="s">
         <v>178</v>
       </c>
@@ -4526,7 +4696,7 @@
       </c>
       <c r="F158" s="5"/>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" hidden="1">
       <c r="A159" s="5" t="s">
         <v>178</v>
       </c>
@@ -4542,7 +4712,7 @@
       </c>
       <c r="F159" s="5"/>
     </row>
-    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" hidden="1">
       <c r="A160" s="5" t="s">
         <v>178</v>
       </c>
@@ -4558,7 +4728,7 @@
       </c>
       <c r="F160" s="5"/>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" hidden="1">
       <c r="A161" s="5" t="s">
         <v>178</v>
       </c>
@@ -4574,7 +4744,7 @@
       </c>
       <c r="F161" s="5"/>
     </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" hidden="1">
       <c r="A162" s="5" t="s">
         <v>178</v>
       </c>
@@ -4590,7 +4760,7 @@
       </c>
       <c r="F162" s="5"/>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" hidden="1">
       <c r="A163" s="5" t="s">
         <v>178</v>
       </c>
@@ -4606,7 +4776,7 @@
       </c>
       <c r="F163" s="5"/>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" hidden="1">
       <c r="A164" s="5" t="s">
         <v>178</v>
       </c>
@@ -4626,7 +4796,7 @@
   <autoFilter ref="A1:F164" xr:uid="{ED56F733-C473-4479-9885-B4D7B8ADB1BF}">
     <filterColumn colId="0">
       <filters>
-        <filter val="CurrencyConv"/>
+        <filter val="MedicinePrice"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4635,6 +4805,223 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15620030-597F-4032-A3AA-B1DEB0BD6241}">
+  <dimension ref="A2:C49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>233</v>
+      </c>
+      <c r="B14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>238</v>
+      </c>
+      <c r="B21" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>239</v>
+      </c>
+      <c r="B22" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>244</v>
+      </c>
+      <c r="B24" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>244</v>
+      </c>
+      <c r="B25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>244</v>
+      </c>
+      <c r="B26" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="B31" t="s">
+        <v>252</v>
+      </c>
+      <c r="C31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="B32" t="s">
+        <v>253</v>
+      </c>
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="B33" t="s">
+        <v>254</v>
+      </c>
+      <c r="C33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="B34" t="s">
+        <v>255</v>
+      </c>
+      <c r="C34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="B39" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="18" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32359F6-8FC7-4B9E-958B-6733E0C0B68B}">
   <dimension ref="A2:C29"/>
   <sheetViews>
@@ -4642,51 +5029,51 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1">
       <c r="A2" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1">
       <c r="B3" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="B4" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="B5" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="B6" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="B7" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="B8" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -4697,7 +5084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="B11" s="5" t="s">
         <v>38</v>
       </c>
@@ -4705,7 +5092,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="B12" s="5" t="s">
         <v>38</v>
       </c>
@@ -4713,7 +5100,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="B13" s="5" t="s">
         <v>38</v>
       </c>
@@ -4721,7 +5108,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
@@ -4729,7 +5116,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="B15" s="5" t="s">
         <v>38</v>
       </c>
@@ -4737,7 +5124,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="B16" s="5" t="s">
         <v>38</v>
       </c>
@@ -4745,7 +5132,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3">
       <c r="B17" s="5" t="s">
         <v>42</v>
       </c>
@@ -4753,7 +5140,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3">
       <c r="B18" s="7" t="s">
         <v>42</v>
       </c>
@@ -4761,7 +5148,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3">
       <c r="B19" s="5" t="s">
         <v>42</v>
       </c>
@@ -4769,7 +5156,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3">
       <c r="B20" s="5" t="s">
         <v>42</v>
       </c>
@@ -4777,7 +5164,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3">
       <c r="B21" s="5" t="s">
         <v>42</v>
       </c>
@@ -4785,7 +5172,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3">
       <c r="B22" s="5" t="s">
         <v>42</v>
       </c>
@@ -4793,7 +5180,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3">
       <c r="B23" s="7" t="s">
         <v>42</v>
       </c>
@@ -4801,7 +5188,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3">
       <c r="B24" s="7" t="s">
         <v>42</v>
       </c>
@@ -4809,7 +5196,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3">
       <c r="B25" s="7" t="s">
         <v>42</v>
       </c>
@@ -4817,7 +5204,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3">
       <c r="B26" s="7" t="s">
         <v>58</v>
       </c>
@@ -4825,7 +5212,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3">
       <c r="B27" s="7" t="s">
         <v>58</v>
       </c>
@@ -4833,7 +5220,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3">
       <c r="B28" s="7" t="s">
         <v>58</v>
       </c>
@@ -4841,7 +5228,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3">
       <c r="B29" s="7" t="s">
         <v>58</v>
       </c>
@@ -4853,7 +5240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FCAFE7-816B-4CEC-870F-0831C89AC35D}">
   <dimension ref="B2:E10"/>
   <sheetViews>
@@ -4861,35 +5248,35 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="18.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" ht="15.75" thickBot="1"/>
+    <row r="5" spans="2:5" ht="30" customHeight="1" thickBot="1">
       <c r="E5" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="18" customHeight="1">
       <c r="E6"/>
     </row>
-    <row r="7" spans="2:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" ht="18" customHeight="1" thickBot="1">
       <c r="E7"/>
     </row>
-    <row r="8" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" ht="21.75" customHeight="1" thickBot="1">
       <c r="E8" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="24" customHeight="1" thickBot="1"/>
+    <row r="10" spans="2:5" ht="25.5" customHeight="1" thickBot="1">
       <c r="E10" s="8" t="s">
         <v>188</v>
       </c>
@@ -4899,7 +5286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F312F2C-659B-455B-86FB-3F8E8752A32B}">
   <dimension ref="C2:C13"/>
   <sheetViews>
@@ -4907,51 +5294,51 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:3" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:3" ht="15.75" thickBot="1">
       <c r="C3" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:3" ht="15.75" thickBot="1">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:3" ht="15.75" thickBot="1">
       <c r="C5" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:3" ht="15.75" thickBot="1">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:3" ht="15.75" thickBot="1">
       <c r="C7" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:3" ht="15.75" thickBot="1">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:3" ht="15.75" thickBot="1">
       <c r="C9" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:3" ht="15.75" thickBot="1">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:3" ht="15.75" thickBot="1">
       <c r="C11" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:3" ht="15.75" thickBot="1"/>
+    <row r="13" spans="3:3" ht="15.75" thickBot="1">
       <c r="C13" s="8" t="s">
         <v>199</v>
       </c>
@@ -4961,19 +5348,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7613B243-9037-4598-8398-0BBE211C1614}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F552D3-184E-45E8-947E-31C55B949583}">
   <dimension ref="B2:I22"/>
   <sheetViews>
@@ -4981,7 +5368,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
@@ -4991,30 +5378,30 @@
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9">
       <c r="B2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9">
       <c r="B3" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>189</v>
       </c>
       <c r="C5" s="10"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9">
       <c r="B8" s="9" t="s">
         <v>190</v>
       </c>
@@ -5034,7 +5421,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9">
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
@@ -5049,84 +5436,84 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>

</xml_diff>

<commit_message>
command to upload csv files
</commit_message>
<xml_diff>
--- a/priceTrackerTables.xlsx
+++ b/priceTrackerTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\django\priceTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576D11BB-9C7C-4E56-87C7-DBC354212CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C70B68E-A41B-4DED-BC31-82DE466E93EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A0984463-1538-4671-813D-D6CC57BDADC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A0984463-1538-4671-813D-D6CC57BDADC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="price_menu" sheetId="5" r:id="rId6"/>
     <sheet name="food" sheetId="7" r:id="rId7"/>
     <sheet name="food_prices" sheetId="6" r:id="rId8"/>
+    <sheet name="frontend_eval" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fields!$A$1:$F$164</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="288">
   <si>
     <t>Main</t>
   </si>
@@ -654,18 +655,12 @@
     <t>Price area</t>
   </si>
   <si>
-    <t>HomeType</t>
-  </si>
-  <si>
     <t>PriceType</t>
   </si>
   <si>
     <t>UnitType</t>
   </si>
   <si>
-    <t>Usage</t>
-  </si>
-  <si>
     <t>ActivityLog</t>
   </si>
   <si>
@@ -829,6 +824,90 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Front end</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Charts</t>
+  </si>
+  <si>
+    <t>App building</t>
+  </si>
+  <si>
+    <t>Learning Curve</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>advanced</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>App Gyver</t>
+  </si>
+  <si>
+    <t>remote</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>easy</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>App Smith</t>
+  </si>
+  <si>
+    <t>perfect</t>
+  </si>
+  <si>
+    <t>Bubble</t>
+  </si>
+  <si>
+    <t>intermediate</t>
+  </si>
+  <si>
+    <t>unfit</t>
+  </si>
+  <si>
+    <t>complex</t>
+  </si>
+  <si>
+    <t>HouseType</t>
+  </si>
+  <si>
+    <t>HousePriceSource</t>
+  </si>
+  <si>
+    <t>ResourceUsage</t>
+  </si>
+  <si>
+    <t>Admin created</t>
+  </si>
+  <si>
+    <t>Activity</t>
   </si>
 </sst>
 </file>
@@ -1324,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C77FEE-F832-43C4-A92B-CA75BC9DC9BF}">
-  <dimension ref="B1:M34"/>
+  <dimension ref="B1:N34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1336,15 +1415,16 @@
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13">
+    <row r="1" spans="2:14">
       <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>5</v>
@@ -1353,36 +1433,39 @@
         <v>201</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="2:13">
+    <row r="2" spans="2:14">
       <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>6</v>
@@ -1390,12 +1473,10 @@
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="14">
-        <v>1</v>
-      </c>
       <c r="J2" s="14">
         <v>1</v>
       </c>
@@ -1408,8 +1489,11 @@
       <c r="M2" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:13">
+      <c r="N2" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14">
       <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
@@ -1421,47 +1505,49 @@
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
-      <c r="G3" s="14">
-        <v>1</v>
-      </c>
-      <c r="H3" s="14" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="14">
+        <v>1</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="14"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
-      <c r="M3" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13">
+      <c r="M3" s="14"/>
+      <c r="N3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
       <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
-      <c r="G4" s="14">
-        <v>1</v>
-      </c>
-      <c r="H4" s="14" t="s">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14">
+        <v>1</v>
+      </c>
+      <c r="I4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="14"/>
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
       <c r="L4" s="14"/>
-      <c r="M4" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13">
+      <c r="M4" s="14"/>
+      <c r="N4" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14">
       <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
@@ -1472,18 +1558,19 @@
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="14"/>
+      <c r="I5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
-      <c r="M5" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13">
+      <c r="M5" s="14"/>
+      <c r="N5" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14">
       <c r="B6" s="14" t="s">
         <v>14</v>
       </c>
@@ -1493,21 +1580,22 @@
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
-      <c r="G6" s="14">
-        <v>1</v>
-      </c>
-      <c r="H6" s="14" t="s">
+      <c r="G6" s="14"/>
+      <c r="H6" s="14">
+        <v>1</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13">
+      <c r="M6" s="14"/>
+      <c r="N6" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
       <c r="B7" s="14" t="s">
         <v>18</v>
       </c>
@@ -1523,11 +1611,12 @@
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
-      <c r="M7" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13">
+      <c r="M7" s="14"/>
+      <c r="N7" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
       <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
@@ -1543,11 +1632,12 @@
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
-      <c r="M8" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13">
+      <c r="M8" s="14"/>
+      <c r="N8" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
       <c r="B9" s="14" t="s">
         <v>24</v>
       </c>
@@ -1559,19 +1649,20 @@
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
-      <c r="G9" s="14">
-        <v>1</v>
-      </c>
-      <c r="H9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14">
+        <v>1</v>
+      </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13">
+      <c r="M9" s="14"/>
+      <c r="N9" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14">
       <c r="B10" s="14" t="s">
         <v>26</v>
       </c>
@@ -1581,21 +1672,22 @@
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="14">
-        <v>1</v>
-      </c>
-      <c r="H10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14">
+        <v>1</v>
+      </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
-      <c r="M10" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13">
+      <c r="M10" s="14"/>
+      <c r="N10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
       <c r="B11" s="15" t="s">
-        <v>207</v>
+        <v>287</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
@@ -1606,20 +1698,23 @@
       <c r="G11" s="15">
         <v>1</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15">
-        <v>1</v>
-      </c>
-      <c r="K11" s="15"/>
+      <c r="H11" s="15">
+        <v>1</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15">
+        <v>1</v>
+      </c>
       <c r="L11" s="15"/>
-      <c r="M11" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13">
+      <c r="M11" s="15"/>
+      <c r="N11" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
       <c r="B12" s="15" t="s">
         <v>201</v>
       </c>
@@ -1629,23 +1724,24 @@
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="15">
-        <v>1</v>
-      </c>
-      <c r="H12" s="15" t="s">
+      <c r="G12" s="15"/>
+      <c r="H12" s="15">
+        <v>1</v>
+      </c>
+      <c r="I12" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15">
-        <v>1</v>
-      </c>
-      <c r="K12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15">
+        <v>1</v>
+      </c>
       <c r="L12" s="15"/>
-      <c r="M12" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13">
+      <c r="M12" s="15"/>
+      <c r="N12" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14">
       <c r="B13" s="15" t="s">
         <v>7</v>
       </c>
@@ -1655,23 +1751,24 @@
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="15">
-        <v>1</v>
-      </c>
-      <c r="H13" s="15" t="s">
+      <c r="G13" s="15"/>
+      <c r="H13" s="15">
+        <v>1</v>
+      </c>
+      <c r="I13" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
-      <c r="M13" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13">
+      <c r="M13" s="15"/>
+      <c r="N13" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14">
       <c r="B14" s="15" t="s">
-        <v>203</v>
+        <v>284</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
@@ -1679,25 +1776,26 @@
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="15">
-        <v>1</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15">
-        <v>1</v>
-      </c>
-      <c r="K14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15">
+        <v>1</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15">
+        <v>1</v>
+      </c>
       <c r="L14" s="15"/>
-      <c r="M14" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13">
+      <c r="M14" s="15"/>
+      <c r="N14" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14">
       <c r="B15" s="15" t="s">
-        <v>145</v>
+        <v>283</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
@@ -1705,25 +1803,26 @@
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="15">
-        <v>1</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15">
-        <v>1</v>
-      </c>
-      <c r="K15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15">
+        <v>1</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15">
+        <v>1</v>
+      </c>
       <c r="L15" s="15"/>
-      <c r="M15" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13">
+      <c r="M15" s="15"/>
+      <c r="N15" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14">
       <c r="B16" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
@@ -1731,25 +1830,26 @@
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
-      <c r="G16" s="15">
-        <v>1</v>
-      </c>
-      <c r="H16" s="15" t="s">
+      <c r="G16" s="15"/>
+      <c r="H16" s="15">
+        <v>1</v>
+      </c>
+      <c r="I16" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15">
-        <v>1</v>
-      </c>
-      <c r="K16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15">
+        <v>1</v>
+      </c>
       <c r="L16" s="15"/>
-      <c r="M16" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13">
+      <c r="M16" s="15"/>
+      <c r="N16" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
       <c r="B17" s="15" t="s">
-        <v>25</v>
+        <v>285</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
@@ -1757,23 +1857,26 @@
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
-      <c r="G17" s="15">
-        <v>1</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="I17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15">
+        <v>1</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>36</v>
+      </c>
       <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
+      <c r="K17" s="15">
+        <v>1</v>
+      </c>
       <c r="L17" s="15"/>
-      <c r="M17" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13">
+      <c r="M17" s="15"/>
+      <c r="N17" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
       <c r="B18" s="15" t="s">
-        <v>205</v>
+        <v>25</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
@@ -1781,25 +1884,24 @@
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="15">
-        <v>1</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15">
-        <v>1</v>
-      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15">
+        <v>1</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
-      <c r="M18" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13">
+      <c r="M18" s="15"/>
+      <c r="N18" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
       <c r="B19" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
@@ -1813,13 +1915,14 @@
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
-      <c r="M19" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13">
+      <c r="M19" s="15"/>
+      <c r="N19" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
       <c r="B20" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
@@ -1827,101 +1930,101 @@
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="15">
-        <v>1</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15">
-        <v>1</v>
-      </c>
-      <c r="K20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15">
+        <v>1</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15">
+        <v>1</v>
+      </c>
       <c r="L20" s="15"/>
-      <c r="M20" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13">
+      <c r="M20" s="15"/>
+      <c r="N20" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
       <c r="B21" s="5" t="s">
-        <v>11</v>
+        <v>205</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="5">
-        <v>1</v>
-      </c>
+      <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" s="5"/>
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>210</v>
+      </c>
       <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
+      <c r="K21" s="5">
+        <v>1</v>
+      </c>
       <c r="L21" s="5"/>
-      <c r="M21" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13">
+      <c r="M21" s="5"/>
+      <c r="N21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
       <c r="B22" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="E22" s="5"/>
       <c r="F22" s="5">
         <v>1</v>
       </c>
       <c r="G22" s="5"/>
-      <c r="H22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13">
+      <c r="M22" s="5"/>
+      <c r="N22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
       <c r="B23" s="5" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="5">
-        <v>1</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="5" t="s">
-        <v>214</v>
-      </c>
+      <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
-      <c r="M23" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13">
+      <c r="M23" s="5"/>
+      <c r="N23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
       <c r="B24" s="5" t="s">
-        <v>219</v>
+        <v>13</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
@@ -1930,18 +2033,23 @@
       <c r="E24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="I24" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
-      <c r="M24" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13">
+      <c r="M24" s="5"/>
+      <c r="N24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
       <c r="B25" s="5" t="s">
         <v>16</v>
       </c>
@@ -1961,20 +2069,21 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
-      <c r="M25" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13">
+      <c r="M25" s="5"/>
+      <c r="N25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
       <c r="B26" s="5" t="s">
-        <v>17</v>
+        <v>216</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F26" s="5">
         <v>1</v>
@@ -1985,35 +2094,41 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
-      <c r="M26" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13">
+      <c r="M26" s="5"/>
+      <c r="N26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
       <c r="B27" s="5" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1</v>
+      </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+      <c r="I27" s="5" t="s">
+        <v>212</v>
+      </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
-      <c r="M27" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13">
+      <c r="M27" s="5"/>
+      <c r="N27" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
       <c r="B28" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
@@ -2029,66 +2144,69 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
-      <c r="M28" s="5">
+      <c r="M28" s="5"/>
+      <c r="N28" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:13">
+    <row r="29" spans="2:14">
       <c r="B29" s="5" t="s">
-        <v>222</v>
+        <v>17</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>218</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1</v>
+      </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
-      <c r="M29" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13">
+      <c r="M29" s="5"/>
+      <c r="N29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
       <c r="B30" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="F30" s="5">
-        <v>1</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
-      <c r="M30" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13">
+      <c r="M30" s="5"/>
+      <c r="N30" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
       <c r="B31" s="5" t="s">
-        <v>217</v>
+        <v>170</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>217</v>
+        <v>18</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -2097,13 +2215,14 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
-      <c r="M31" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13">
+      <c r="M31" s="5"/>
+      <c r="N31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14">
       <c r="B32" s="5" t="s">
-        <v>27</v>
+        <v>215</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
@@ -2112,57 +2231,68 @@
       <c r="E32" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F32" s="5">
-        <v>1</v>
-      </c>
+      <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-      <c r="M32" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13">
-      <c r="B33" s="16" t="s">
+      <c r="M32" s="5"/>
+      <c r="N32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14">
+      <c r="B33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F33" s="5">
+        <v>1</v>
+      </c>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14">
+      <c r="B34" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13">
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:M34">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:N34">
     <sortCondition ref="D2:D34"/>
     <sortCondition ref="B2:B34"/>
   </sortState>
@@ -4808,7 +4938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15620030-597F-4032-A3AA-B1DEB0BD6241}">
   <dimension ref="A2:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
@@ -4816,42 +4946,42 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4866,91 +4996,91 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B23" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B24" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B25" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C31" t="s">
         <v>85</v>
@@ -4958,7 +5088,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="B32" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C32" t="s">
         <v>85</v>
@@ -4966,7 +5096,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="B33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C33" t="s">
         <v>85</v>
@@ -4974,7 +5104,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="B34" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C34" t="s">
         <v>116</v>
@@ -4982,37 +5112,37 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="B39" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -5040,7 +5170,7 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1">
@@ -5523,4 +5653,234 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5907808D-391F-4495-BCC3-91693FD270CA}">
+  <dimension ref="B2:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:8">
+      <c r="B2" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>2</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <f>SUM(C9:G9)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>3</v>
+      </c>
+      <c r="G10" s="5">
+        <v>2</v>
+      </c>
+      <c r="H10" s="5">
+        <f>SUM(C10:G10)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>3</v>
+      </c>
+      <c r="F11" s="5">
+        <v>3</v>
+      </c>
+      <c r="G11" s="5">
+        <v>3</v>
+      </c>
+      <c r="H11" s="5">
+        <f>SUM(C11:G11)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>2</v>
+      </c>
+      <c r="H12" s="5">
+        <f>SUM(C12:G12)</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
admin for config classes, db restructure
</commit_message>
<xml_diff>
--- a/priceTrackerTables.xlsx
+++ b/priceTrackerTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\django\priceTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C70B68E-A41B-4DED-BC31-82DE466E93EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA71757A-B957-4204-B322-2B5BED9E3545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A0984463-1538-4671-813D-D6CC57BDADC8}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="289">
   <si>
     <t>Main</t>
   </si>
@@ -908,6 +908,9 @@
   </si>
   <si>
     <t>Activity</t>
+  </si>
+  <si>
+    <t>Language used by each contry</t>
   </si>
 </sst>
 </file>
@@ -1403,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C77FEE-F832-43C4-A92B-CA75BC9DC9BF}">
-  <dimension ref="B1:N34"/>
+  <dimension ref="B1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1672,7 +1675,9 @@
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="G10" s="14">
+        <v>1</v>
+      </c>
       <c r="H10" s="14">
         <v>1</v>
       </c>
@@ -1724,7 +1729,9 @@
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="G12" s="15">
+        <v>1</v>
+      </c>
       <c r="H12" s="15">
         <v>1</v>
       </c>
@@ -1751,7 +1758,9 @@
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="G13" s="15">
+        <v>1</v>
+      </c>
       <c r="H13" s="15">
         <v>1</v>
       </c>
@@ -1776,7 +1785,9 @@
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="G14" s="15">
+        <v>1</v>
+      </c>
       <c r="H14" s="15">
         <v>1</v>
       </c>
@@ -1803,7 +1814,9 @@
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="G15" s="15">
+        <v>1</v>
+      </c>
       <c r="H15" s="15">
         <v>1</v>
       </c>
@@ -1822,7 +1835,7 @@
     </row>
     <row r="16" spans="2:14">
       <c r="B16" s="15" t="s">
-        <v>203</v>
+        <v>73</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
@@ -1830,26 +1843,24 @@
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="G16" s="15">
+        <v>1</v>
+      </c>
       <c r="H16" s="15">
         <v>1</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>30</v>
+        <v>288</v>
       </c>
       <c r="J16" s="15"/>
-      <c r="K16" s="15">
-        <v>1</v>
-      </c>
+      <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
-      <c r="N16" s="15">
-        <v>1</v>
-      </c>
+      <c r="N16" s="15"/>
     </row>
     <row r="17" spans="2:14">
       <c r="B17" s="15" t="s">
-        <v>285</v>
+        <v>203</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
@@ -1857,12 +1868,14 @@
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="G17" s="15">
+        <v>1</v>
+      </c>
       <c r="H17" s="15">
         <v>1</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15">
@@ -1876,7 +1889,7 @@
     </row>
     <row r="18" spans="2:14">
       <c r="B18" s="15" t="s">
-        <v>25</v>
+        <v>285</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
@@ -1884,15 +1897,19 @@
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="G18" s="15">
+        <v>1</v>
+      </c>
       <c r="H18" s="15">
         <v>1</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>208</v>
+        <v>36</v>
       </c>
       <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
+      <c r="K18" s="15">
+        <v>1</v>
+      </c>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
       <c r="N18" s="15">
@@ -1901,7 +1918,7 @@
     </row>
     <row r="19" spans="2:14">
       <c r="B19" s="15" t="s">
-        <v>209</v>
+        <v>25</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
@@ -1909,9 +1926,15 @@
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
+      <c r="G19" s="15">
+        <v>1</v>
+      </c>
+      <c r="H19" s="15">
+        <v>1</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>208</v>
+      </c>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
@@ -1922,7 +1945,7 @@
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="15" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
@@ -1930,17 +1953,13 @@
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15">
-        <v>1</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>31</v>
-      </c>
+      <c r="G20" s="15">
+        <v>1</v>
+      </c>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
       <c r="J20" s="15"/>
-      <c r="K20" s="15">
-        <v>1</v>
-      </c>
+      <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
       <c r="N20" s="15">
@@ -1948,51 +1967,53 @@
       </c>
     </row>
     <row r="21" spans="2:14">
-      <c r="B21" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5">
-        <v>1</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5">
-        <v>1</v>
-      </c>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5">
+      <c r="B21" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15">
+        <v>1</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15">
+        <v>1</v>
+      </c>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:14">
       <c r="B22" s="5" t="s">
-        <v>11</v>
+        <v>205</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="5">
-        <v>1</v>
-      </c>
+      <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
       <c r="I22" s="5" t="s">
-        <v>34</v>
+        <v>210</v>
       </c>
       <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+      <c r="K22" s="5">
+        <v>1</v>
+      </c>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="5">
@@ -2001,71 +2022,71 @@
     </row>
     <row r="23" spans="2:14">
       <c r="B23" s="5" t="s">
-        <v>219</v>
+        <v>11</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="I23" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:14">
       <c r="B24" s="5" t="s">
-        <v>13</v>
+        <v>219</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="5">
-        <v>1</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
-      <c r="I24" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:14">
       <c r="B25" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F25" s="5">
         <v>1</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="I25" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -2076,14 +2097,14 @@
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="5" t="s">
-        <v>216</v>
+        <v>16</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>215</v>
+        <v>14</v>
       </c>
       <c r="F26" s="5">
         <v>1</v>
@@ -2101,23 +2122,21 @@
     </row>
     <row r="27" spans="2:14">
       <c r="B27" s="5" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>39</v>
+        <v>215</v>
       </c>
       <c r="F27" s="5">
         <v>1</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="5" t="s">
-        <v>212</v>
-      </c>
+      <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -2128,41 +2147,43 @@
     </row>
     <row r="28" spans="2:14">
       <c r="B28" s="5" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F28" s="5">
+        <v>1</v>
+      </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
+      <c r="I28" s="5" t="s">
+        <v>212</v>
+      </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:14">
       <c r="B29" s="5" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="F29" s="5">
-        <v>1</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -2171,21 +2192,23 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:14">
       <c r="B30" s="5" t="s">
-        <v>217</v>
+        <v>17</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>218</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -2199,14 +2222,14 @@
     </row>
     <row r="31" spans="2:14">
       <c r="B31" s="5" t="s">
-        <v>170</v>
+        <v>217</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -2222,14 +2245,14 @@
     </row>
     <row r="32" spans="2:14">
       <c r="B32" s="5" t="s">
-        <v>215</v>
+        <v>170</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>215</v>
+        <v>18</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -2245,18 +2268,16 @@
     </row>
     <row r="33" spans="2:14">
       <c r="B33" s="5" t="s">
-        <v>27</v>
+        <v>215</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="F33" s="5">
-        <v>1</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -2269,32 +2290,57 @@
       </c>
     </row>
     <row r="34" spans="2:14">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14">
+      <c r="B35" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16" t="s">
+      <c r="C35" s="16"/>
+      <c r="D35" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16" t="s">
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16">
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:N34">
-    <sortCondition ref="D2:D34"/>
-    <sortCondition ref="B2:B34"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:N35">
+    <sortCondition ref="D2:D35"/>
+    <sortCondition ref="B2:B35"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>